<commit_message>
Update edited session - 2025-08-14T07:39:17.662Z - Cache Bust ID: 1755157157662d93robq21
</commit_message>
<xml_diff>
--- a/log_history/Y1_B2223_Anatomy_checklist1755157078081_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
+++ b/log_history/Y1_B2223_Anatomy_checklist1755157078081_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,7 +424,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>231249</v>
+        <v>232000</v>
       </c>
       <c r="B2" t="str">
         <v>Anatomy</v>
@@ -436,7 +436,7 @@
         <v>10:38:02</v>
       </c>
       <c r="E2" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F2" t="str">
         <v>admin@admin.com</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>232000</v>
+        <v>231999</v>
       </c>
       <c r="B3" t="str">
         <v>Anatomy</v>
@@ -453,10 +453,10 @@
         <v>14/08/2025</v>
       </c>
       <c r="D3" t="str">
-        <v>10:38:02</v>
+        <v>10:38:03</v>
       </c>
       <c r="E3" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F3" t="str">
         <v>admin@admin.com</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>231999</v>
+        <v>232001</v>
       </c>
       <c r="B4" t="str">
         <v>Anatomy</v>
@@ -476,7 +476,7 @@
         <v>10:38:03</v>
       </c>
       <c r="E4" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F4" t="str">
         <v>admin@admin.com</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>232001</v>
+        <v>235000</v>
       </c>
       <c r="B5" t="str">
         <v>Anatomy</v>
@@ -496,7 +496,7 @@
         <v>10:38:03</v>
       </c>
       <c r="E5" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F5" t="str">
         <v>admin@admin.com</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>235000</v>
+        <v>235010</v>
       </c>
       <c r="B6" t="str">
         <v>Anatomy</v>
@@ -513,10 +513,10 @@
         <v>14/08/2025</v>
       </c>
       <c r="D6" t="str">
-        <v>10:38:03</v>
+        <v>10:38:05</v>
       </c>
       <c r="E6" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F6" t="str">
         <v>admin@admin.com</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>235010</v>
+        <v>235020</v>
       </c>
       <c r="B7" t="str">
         <v>Anatomy</v>
@@ -536,35 +536,15 @@
         <v>10:38:05</v>
       </c>
       <c r="E7" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F7" t="str">
         <v>admin@admin.com</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>235020</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C8" t="str">
-        <v>14/08/2025</v>
-      </c>
-      <c r="D8" t="str">
-        <v>10:38:05</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Selection</v>
-      </c>
-      <c r="F8" t="str">
-        <v>admin@admin.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-08-17T15:25:25.879Z - Cache Bust ID: 1755444325879vlwza4itw
</commit_message>
<xml_diff>
--- a/log_history/Y1_B2223_Anatomy_checklist1755157078081_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
+++ b/log_history/Y1_B2223_Anatomy_checklist1755157078081_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -522,29 +522,9 @@
         <v>admin@admin.com</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>235020</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C7" t="str">
-        <v>14/08/2025</v>
-      </c>
-      <c r="D7" t="str">
-        <v>10:38:05</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F7" t="str">
-        <v>admin@admin.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-08-17T15:32:40.394Z - Cache Bust: 1755444760394
</commit_message>
<xml_diff>
--- a/log_history/Y1_B2223_Anatomy_checklist1755157078081_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
+++ b/log_history/Y1_B2223_Anatomy_checklist1755157078081_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Anatomy" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,7 +464,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>232001</v>
+        <v>235000</v>
       </c>
       <c r="B4" t="str">
         <v>Anatomy</v>
@@ -479,52 +479,12 @@
         <v>Scan</v>
       </c>
       <c r="F4" t="str">
-        <v>admin@admin.com</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>235000</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C5" t="str">
-        <v>14/08/2025</v>
-      </c>
-      <c r="D5" t="str">
-        <v>10:38:03</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F5" t="str">
-        <v>admin@admin.com</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>235010</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C6" t="str">
-        <v>14/08/2025</v>
-      </c>
-      <c r="D6" t="str">
-        <v>10:38:05</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F6" t="str">
         <v>admin@admin.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>